<commit_message>
latest update on corwin spreadgen. Code to analyze resonances in depth
</commit_message>
<xml_diff>
--- a/masks/code/diplexer_FINAL_AT_edits.xlsx
+++ b/masks/code/diplexer_FINAL_AT_edits.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97">
+  <si>
+    <t>AGA Marks</t>
+  </si>
+  <si>
+    <t>TVPA</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Alignment Layer</t>
+  </si>
   <si>
     <t>Alternate Array Layout</t>
   </si>
@@ -53,12 +74,6 @@
     <t>Cell name</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>xl</t>
   </si>
   <si>
@@ -84,9 +99,6 @@
   </si>
   <si>
     <t>R</t>
-  </si>
-  <si>
-    <t>Alignment Layer</t>
   </si>
   <si>
     <t>Anodize_DC2_scaled</t>
@@ -666,21 +678,21 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="17"/>
-    <col customWidth="1" max="2" min="2" width="6"/>
+    <col customWidth="1" max="2" min="2" width="11"/>
     <col customWidth="1" max="3" min="3" width="30"/>
     <col customWidth="1" max="4" min="4" width="8"/>
     <col customWidth="1" max="5" min="5" width="8"/>
     <col customWidth="1" max="6" min="6" width="8"/>
-    <col customWidth="1" max="7" min="7" width="8"/>
-    <col customWidth="1" max="8" min="8" width="22"/>
-    <col customWidth="1" max="9" min="9" width="21"/>
-    <col customWidth="1" max="10" min="10" width="22"/>
-    <col customWidth="1" max="11" min="11" width="22"/>
+    <col customWidth="1" max="7" min="7" width="17"/>
+    <col customWidth="1" max="8" min="8" width="10"/>
+    <col customWidth="1" max="9" min="9" width="9"/>
+    <col customWidth="1" max="10" min="10" width="9"/>
+    <col customWidth="1" max="11" min="11" width="9"/>
     <col customWidth="1" max="12" min="12" width="6"/>
-    <col customWidth="1" max="13" min="13" width="11"/>
-    <col customWidth="1" max="14" min="14" width="21"/>
-    <col customWidth="1" max="15" min="15" width="21"/>
-    <col customWidth="1" max="16" min="16" width="21"/>
+    <col customWidth="1" max="13" min="13" width="9"/>
+    <col customWidth="1" max="14" min="14" width="9"/>
+    <col customWidth="1" max="15" min="15" width="9"/>
+    <col customWidth="1" max="16" min="16" width="9"/>
     <col customWidth="1" max="17" min="17" width="6"/>
     <col customWidth="1" max="18" min="18" width="6"/>
     <col customWidth="1" max="19" min="19" width="11"/>
@@ -695,13 +707,235 @@
     <row r="1" spans="1:25"/>
     <row r="2" spans="1:25"/>
     <row r="3" spans="1:25"/>
-    <row r="4" spans="1:25"/>
-    <row r="5" spans="1:25"/>
-    <row r="6" spans="1:25"/>
-    <row r="7" spans="1:25"/>
-    <row r="8" spans="1:25"/>
-    <row r="9" spans="1:25"/>
-    <row r="10" spans="1:25"/>
+    <row r="4" spans="1:25">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="n"/>
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
+      <c r="T4" s="1" t="n"/>
+      <c r="U4" s="1" t="n"/>
+      <c r="V4" s="1" t="n"/>
+      <c r="W4" s="1" t="n"/>
+      <c r="X4" s="1" t="n"/>
+      <c r="Y4" s="1" t="n"/>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="n"/>
+      <c r="K5" s="1" t="n"/>
+      <c r="L5" s="1" t="n"/>
+      <c r="M5" s="1" t="n"/>
+      <c r="N5" s="1" t="n"/>
+      <c r="O5" s="1" t="n"/>
+      <c r="P5" s="1" t="n"/>
+      <c r="Q5" s="1" t="n"/>
+      <c r="R5" s="1" t="n"/>
+      <c r="S5" s="1" t="n"/>
+      <c r="T5" s="1" t="n"/>
+      <c r="U5" s="1" t="n"/>
+      <c r="V5" s="1" t="n"/>
+      <c r="W5" s="1" t="n"/>
+      <c r="X5" s="1" t="n"/>
+      <c r="Y5" s="1" t="n"/>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>-0.225</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n"/>
+      <c r="K6" s="1" t="n"/>
+      <c r="L6" s="1" t="n"/>
+      <c r="M6" s="1" t="n"/>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="n"/>
+      <c r="P6" s="1" t="n"/>
+      <c r="Q6" s="1" t="n"/>
+      <c r="R6" s="1" t="n"/>
+      <c r="S6" s="1" t="n"/>
+      <c r="T6" s="1" t="n"/>
+      <c r="U6" s="1" t="n"/>
+      <c r="V6" s="1" t="n"/>
+      <c r="W6" s="1" t="n"/>
+      <c r="X6" s="1" t="n"/>
+      <c r="Y6" s="1" t="n"/>
+    </row>
+    <row r="7" spans="1:25">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>-0.125</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="1" t="n"/>
+      <c r="L7" s="1" t="n"/>
+      <c r="M7" s="1" t="n"/>
+      <c r="N7" s="1" t="n"/>
+      <c r="O7" s="1" t="n"/>
+      <c r="P7" s="1" t="n"/>
+      <c r="Q7" s="1" t="n"/>
+      <c r="R7" s="1" t="n"/>
+      <c r="S7" s="1" t="n"/>
+      <c r="T7" s="1" t="n"/>
+      <c r="U7" s="1" t="n"/>
+      <c r="V7" s="1" t="n"/>
+      <c r="W7" s="1" t="n"/>
+      <c r="X7" s="1" t="n"/>
+      <c r="Y7" s="1" t="n"/>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="n"/>
+      <c r="I8" s="1" t="n"/>
+      <c r="J8" s="1" t="n"/>
+      <c r="K8" s="1" t="n"/>
+      <c r="L8" s="1" t="n"/>
+      <c r="M8" s="1" t="n"/>
+      <c r="N8" s="1" t="n"/>
+      <c r="O8" s="1" t="n"/>
+      <c r="P8" s="1" t="n"/>
+      <c r="Q8" s="1" t="n"/>
+      <c r="R8" s="1" t="n"/>
+      <c r="S8" s="1" t="n"/>
+      <c r="T8" s="1" t="n"/>
+      <c r="U8" s="1" t="n"/>
+      <c r="V8" s="1" t="n"/>
+      <c r="W8" s="1" t="n"/>
+      <c r="X8" s="1" t="n"/>
+      <c r="Y8" s="1" t="n"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
+      <c r="I9" s="1" t="n"/>
+      <c r="J9" s="1" t="n"/>
+      <c r="K9" s="1" t="n"/>
+      <c r="L9" s="1" t="n"/>
+      <c r="M9" s="1" t="n"/>
+      <c r="N9" s="1" t="n"/>
+      <c r="O9" s="1" t="n"/>
+      <c r="P9" s="1" t="n"/>
+      <c r="Q9" s="1" t="n"/>
+      <c r="R9" s="1" t="n"/>
+      <c r="S9" s="1" t="n"/>
+      <c r="T9" s="1" t="n"/>
+      <c r="U9" s="1" t="n"/>
+      <c r="V9" s="1" t="n"/>
+      <c r="W9" s="1" t="n"/>
+      <c r="X9" s="1" t="n"/>
+      <c r="Y9" s="1" t="n"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
+      <c r="E10" s="1" t="n"/>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
+      <c r="H10" s="1" t="n"/>
+      <c r="I10" s="1" t="n"/>
+      <c r="J10" s="1" t="n"/>
+      <c r="K10" s="1" t="n"/>
+      <c r="L10" s="1" t="n"/>
+      <c r="M10" s="1" t="n"/>
+      <c r="N10" s="1" t="n"/>
+      <c r="O10" s="1" t="n"/>
+      <c r="P10" s="1" t="n"/>
+      <c r="Q10" s="1" t="n"/>
+      <c r="R10" s="1" t="n"/>
+      <c r="S10" s="1" t="n"/>
+      <c r="T10" s="1" t="n"/>
+      <c r="U10" s="1" t="n"/>
+      <c r="V10" s="1" t="n"/>
+      <c r="W10" s="1" t="n"/>
+      <c r="X10" s="1" t="n"/>
+      <c r="Y10" s="1" t="n"/>
+    </row>
     <row r="11" spans="1:25">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n"/>
@@ -750,7 +984,7 @@
       <c r="R12" s="1" t="n"/>
       <c r="S12" s="1" t="n"/>
       <c r="T12" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:25">
@@ -758,116 +992,116 @@
       <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L13" s="1" t="n"/>
       <c r="M13" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q13" s="1" t="n"/>
       <c r="R13" s="1" t="n"/>
       <c r="S13" s="1" t="n"/>
       <c r="T13" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="L14" s="1" t="n"/>
       <c r="M14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="n"/>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>-2.9</v>
@@ -895,23 +1129,23 @@
       </c>
       <c r="L15" s="1" t="n"/>
       <c r="M15" s="1" t="n">
-        <v>-54.6</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>-56.4</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>51.7</v>
+        <v>-2.9</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>67.09999999999999</v>
+        <v>10.7</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="R15" s="1" t="n"/>
       <c r="S15" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T15" s="1" t="n">
         <v>15</v>
@@ -920,10 +1154,10 @@
         <v>2</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W15" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X15" s="1" t="n">
         <v>7.8</v>
@@ -934,11 +1168,11 @@
     </row>
     <row r="16" spans="1:25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="n"/>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -966,16 +1200,16 @@
       </c>
       <c r="L16" s="1" t="n"/>
       <c r="M16" s="1" t="n">
-        <v>-45.3</v>
+        <v>-8.835000000000001</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>-48.387</v>
+        <v>-11.922</v>
       </c>
       <c r="O16" s="1" t="n">
-        <v>45.3</v>
+        <v>8.835000000000001</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>48.387</v>
+        <v>11.922</v>
       </c>
       <c r="Q16" s="1" t="n"/>
       <c r="R16" s="1" t="n"/>
@@ -987,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="V16" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W16" s="1" t="n">
         <v>0</v>
@@ -1001,11 +1235,11 @@
     </row>
     <row r="17" spans="1:25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="n"/>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -1068,11 +1302,11 @@
     </row>
     <row r="18" spans="1:25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>-9.300000000000001</v>
@@ -1100,21 +1334,21 @@
       </c>
       <c r="L18" s="1" t="n"/>
       <c r="M18" s="1" t="n">
-        <v>-56.66</v>
+        <v>0</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>-45</v>
+        <v>0</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>47.36</v>
+        <v>-9.300000000000001</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="n"/>
       <c r="S18" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T18" s="1" t="n">
         <v>2</v>
@@ -1123,10 +1357,10 @@
         <v>10</v>
       </c>
       <c r="V18" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W18" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X18" s="1" t="n">
         <v>113.32</v>
@@ -1137,11 +1371,11 @@
     </row>
     <row r="19" spans="1:25">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0</v>
@@ -1169,21 +1403,21 @@
       </c>
       <c r="L19" s="1" t="n"/>
       <c r="M19" s="1" t="n">
-        <v>-46</v>
+        <v>0</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>-56.66</v>
+        <v>0</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>68.66</v>
+        <v>12</v>
       </c>
       <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="n"/>
       <c r="S19" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T19" s="1" t="n">
         <v>7</v>
@@ -1195,7 +1429,7 @@
         <v>-0.5</v>
       </c>
       <c r="W19" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X19" s="1" t="n">
         <v>15</v>
@@ -1206,11 +1440,11 @@
     </row>
     <row r="20" spans="1:25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -1238,21 +1472,21 @@
       </c>
       <c r="L20" s="1" t="n"/>
       <c r="M20" s="1" t="n">
-        <v>-46</v>
+        <v>0</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>-56.66</v>
+        <v>0</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>68.66</v>
+        <v>12</v>
       </c>
       <c r="Q20" s="1" t="n"/>
       <c r="R20" s="1" t="n"/>
       <c r="S20" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T20" s="1" t="n">
         <v>7</v>
@@ -1264,7 +1498,7 @@
         <v>-0.5</v>
       </c>
       <c r="W20" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X20" s="1" t="n">
         <v>15</v>
@@ -1275,11 +1509,11 @@
     </row>
     <row r="21" spans="1:25">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>4.7</v>
@@ -1307,21 +1541,21 @@
       </c>
       <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n">
-        <v>-24.12</v>
+        <v>0</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>111.51</v>
+        <v>0</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>28.82</v>
+        <v>4.7</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>-122.31</v>
+        <v>-10.8</v>
       </c>
       <c r="Q21" s="1" t="n"/>
       <c r="R21" s="1" t="n"/>
       <c r="S21" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T21" s="1" t="n">
         <v>8</v>
@@ -1344,11 +1578,11 @@
     </row>
     <row r="22" spans="1:25">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="n"/>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>1.4</v>
@@ -1376,21 +1610,21 @@
       </c>
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n">
-        <v>-28.72</v>
+        <v>0</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>111.285</v>
+        <v>-0.025</v>
       </c>
       <c r="O22" s="1" t="n">
-        <v>30.12</v>
+        <v>1.4</v>
       </c>
       <c r="P22" s="1" t="n">
-        <v>-122.485</v>
+        <v>-11.175</v>
       </c>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="n"/>
       <c r="S22" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T22" s="1" t="n">
         <v>8</v>
@@ -1402,7 +1636,7 @@
         <v>-0.01</v>
       </c>
       <c r="W22" s="1" t="n">
-        <v>55.505</v>
+        <v>55.355</v>
       </c>
       <c r="X22" s="1" t="n">
         <v>8.199999999999999</v>
@@ -1413,11 +1647,11 @@
     </row>
     <row r="23" spans="1:25">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>-6.5</v>
@@ -1459,7 +1693,7 @@
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="n"/>
       <c r="S23" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T23" s="1" t="n">
         <v>1</v>
@@ -1482,11 +1716,11 @@
     </row>
     <row r="24" spans="1:25">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>-6.3</v>
@@ -1514,21 +1748,21 @@
       </c>
       <c r="L24" s="1" t="n"/>
       <c r="M24" s="1" t="n">
-        <v>106.26</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1" t="n">
-        <v>-56</v>
+        <v>0</v>
       </c>
       <c r="O24" s="1" t="n">
-        <v>-112.56</v>
+        <v>-6.3</v>
       </c>
       <c r="P24" s="1" t="n">
-        <v>62.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="n"/>
       <c r="S24" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T24" s="1" t="n">
         <v>3</v>
@@ -1540,7 +1774,7 @@
         <v>53.88</v>
       </c>
       <c r="W24" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X24" s="1" t="n">
         <v>1.5</v>
@@ -1551,11 +1785,11 @@
     </row>
     <row r="25" spans="1:25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>-6.3</v>
@@ -1583,21 +1817,21 @@
       </c>
       <c r="L25" s="1" t="n"/>
       <c r="M25" s="1" t="n">
-        <v>-109.26</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>-56</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1" t="n">
-        <v>102.96</v>
+        <v>-6.3</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>62.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="n"/>
       <c r="S25" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T25" s="1" t="n">
         <v>3</v>
@@ -1609,7 +1843,7 @@
         <v>-53.88</v>
       </c>
       <c r="W25" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X25" s="1" t="n">
         <v>1.5</v>
@@ -1620,11 +1854,11 @@
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1" t="n"/>
       <c r="C26" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>-4</v>
@@ -1666,7 +1900,7 @@
       <c r="Q26" s="1" t="n"/>
       <c r="R26" s="1" t="n"/>
       <c r="S26" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T26" s="1" t="n">
         <v>1</v>
@@ -1689,11 +1923,11 @@
     </row>
     <row r="27" spans="1:25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="n"/>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>-5.65</v>
@@ -1721,21 +1955,21 @@
       </c>
       <c r="L27" s="1" t="n"/>
       <c r="M27" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O27" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P27" s="1" t="n">
-        <v>21.853</v>
+        <v>-14.612</v>
       </c>
       <c r="Q27" s="1" t="n"/>
       <c r="R27" s="1" t="n"/>
       <c r="S27" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T27" s="1" t="n">
         <v>4</v>
@@ -1744,7 +1978,7 @@
         <v>4</v>
       </c>
       <c r="V27" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W27" s="1" t="n">
         <v>0</v>
@@ -1758,11 +1992,11 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="n"/>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>-5.65</v>
@@ -1790,21 +2024,21 @@
       </c>
       <c r="L28" s="1" t="n"/>
       <c r="M28" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O28" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P28" s="1" t="n">
-        <v>45.453</v>
+        <v>8.988000000000001</v>
       </c>
       <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="n"/>
       <c r="S28" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T28" s="1" t="n">
         <v>4</v>
@@ -1813,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W28" s="1" t="n">
         <v>0</v>
@@ -1827,11 +2061,11 @@
     </row>
     <row r="29" spans="1:25">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="n"/>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>-6.4</v>
@@ -1859,21 +2093,21 @@
       </c>
       <c r="L29" s="1" t="n"/>
       <c r="M29" s="1" t="n">
-        <v>-47.787</v>
+        <v>-11.322</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>41.387</v>
+        <v>4.921999999999999</v>
       </c>
       <c r="P29" s="1" t="n">
-        <v>27.365</v>
+        <v>-9.100000000000001</v>
       </c>
       <c r="Q29" s="1" t="n"/>
       <c r="R29" s="1" t="n"/>
       <c r="S29" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T29" s="1" t="n">
         <v>4</v>
@@ -1882,7 +2116,7 @@
         <v>4</v>
       </c>
       <c r="V29" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W29" s="1" t="n">
         <v>0</v>
@@ -1896,11 +2130,11 @@
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B30" s="1" t="n"/>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D30" s="1" t="n">
         <v>-6.4</v>
@@ -1928,21 +2162,21 @@
       </c>
       <c r="L30" s="1" t="n"/>
       <c r="M30" s="1" t="n">
-        <v>-11.322</v>
+        <v>0</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>-11.803</v>
+        <v>0</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>4.921999999999999</v>
+        <v>-6.4</v>
       </c>
       <c r="P30" s="1" t="n">
-        <v>15.103</v>
+        <v>3.3</v>
       </c>
       <c r="Q30" s="1" t="n"/>
       <c r="R30" s="1" t="n"/>
       <c r="S30" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T30" s="1" t="n">
         <v>2</v>
@@ -1951,10 +2185,10 @@
         <v>2</v>
       </c>
       <c r="V30" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W30" s="1" t="n">
-        <v>-0.003</v>
+        <v>0</v>
       </c>
       <c r="X30" s="1" t="n">
         <v>22.644</v>
@@ -1965,11 +2199,11 @@
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="n"/>
       <c r="C31" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>-6.4</v>
@@ -1997,21 +2231,21 @@
       </c>
       <c r="L31" s="1" t="n"/>
       <c r="M31" s="1" t="n">
-        <v>-11.322</v>
+        <v>0</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>-11.809</v>
+        <v>-0.006</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>4.921999999999999</v>
+        <v>-6.4</v>
       </c>
       <c r="P31" s="1" t="n">
-        <v>15.809</v>
+        <v>4.006</v>
       </c>
       <c r="Q31" s="1" t="n"/>
       <c r="R31" s="1" t="n"/>
       <c r="S31" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T31" s="1" t="n">
         <v>2</v>
@@ -2020,10 +2254,10 @@
         <v>2</v>
       </c>
       <c r="V31" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W31" s="1" t="n">
-        <v>-0.003</v>
+        <v>0</v>
       </c>
       <c r="X31" s="1" t="n">
         <v>22.644</v>
@@ -2034,11 +2268,11 @@
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="n"/>
       <c r="C32" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D32" s="1" t="n">
         <v>-4.5</v>
@@ -2066,21 +2300,21 @@
       </c>
       <c r="L32" s="1" t="n"/>
       <c r="M32" s="1" t="n">
-        <v>-28.72</v>
+        <v>0</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>111.31</v>
+        <v>0</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>24.22</v>
+        <v>-4.5</v>
       </c>
       <c r="P32" s="1" t="n">
-        <v>-122.61</v>
+        <v>-11.3</v>
       </c>
       <c r="Q32" s="1" t="n"/>
       <c r="R32" s="1" t="n"/>
       <c r="S32" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T32" s="1" t="n">
         <v>8</v>
@@ -2092,7 +2326,7 @@
         <v>-0.01</v>
       </c>
       <c r="W32" s="1" t="n">
-        <v>55.505</v>
+        <v>55.355</v>
       </c>
       <c r="X32" s="1" t="n">
         <v>8.199999999999999</v>
@@ -2103,11 +2337,11 @@
     </row>
     <row r="33" spans="1:25">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1" t="n"/>
       <c r="C33" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1" t="n">
         <v>-4.929</v>
@@ -2149,7 +2383,7 @@
       <c r="Q33" s="1" t="n"/>
       <c r="R33" s="1" t="n"/>
       <c r="S33" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T33" s="1" t="n">
         <v>1</v>
@@ -2172,11 +2406,11 @@
     </row>
     <row r="34" spans="1:25">
       <c r="A34" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D34" s="1" t="n">
         <v>-3.73</v>
@@ -2218,7 +2452,7 @@
       <c r="Q34" s="1" t="n"/>
       <c r="R34" s="1" t="n"/>
       <c r="S34" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T34" s="1" t="n">
         <v>1</v>
@@ -2241,11 +2475,11 @@
     </row>
     <row r="35" spans="1:25">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D35" s="1" t="n">
         <v>-2.33</v>
@@ -2287,7 +2521,7 @@
       <c r="Q35" s="1" t="n"/>
       <c r="R35" s="1" t="n"/>
       <c r="S35" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T35" s="1" t="n">
         <v>1</v>
@@ -2310,11 +2544,11 @@
     </row>
     <row r="36" spans="1:25">
       <c r="A36" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B36" s="1" t="n"/>
       <c r="C36" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>-0.93</v>
@@ -2356,7 +2590,7 @@
       <c r="Q36" s="1" t="n"/>
       <c r="R36" s="1" t="n"/>
       <c r="S36" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T36" s="1" t="n">
         <v>1</v>
@@ -2379,11 +2613,11 @@
     </row>
     <row r="37" spans="1:25">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="n"/>
       <c r="C37" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>0.47</v>
@@ -2425,7 +2659,7 @@
       <c r="Q37" s="1" t="n"/>
       <c r="R37" s="1" t="n"/>
       <c r="S37" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T37" s="1" t="n">
         <v>1</v>
@@ -2448,11 +2682,11 @@
     </row>
     <row r="38" spans="1:25">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="n">
         <v>1.87</v>
@@ -2494,7 +2728,7 @@
       <c r="Q38" s="1" t="n"/>
       <c r="R38" s="1" t="n"/>
       <c r="S38" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T38" s="1" t="n">
         <v>1</v>
@@ -2517,11 +2751,11 @@
     </row>
     <row r="39" spans="1:25">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1" t="n"/>
       <c r="C39" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>3.27</v>
@@ -2563,7 +2797,7 @@
       <c r="Q39" s="1" t="n"/>
       <c r="R39" s="1" t="n"/>
       <c r="S39" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T39" s="1" t="n">
         <v>1</v>
@@ -2586,11 +2820,11 @@
     </row>
     <row r="40" spans="1:25">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="n"/>
       <c r="C40" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>4.77</v>
@@ -2632,7 +2866,7 @@
       <c r="Q40" s="1" t="n"/>
       <c r="R40" s="1" t="n"/>
       <c r="S40" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T40" s="1" t="n">
         <v>1</v>
@@ -2655,11 +2889,11 @@
     </row>
     <row r="41" spans="1:25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="n"/>
       <c r="C41" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>-6.4</v>
@@ -2687,21 +2921,21 @@
       </c>
       <c r="L41" s="1" t="n"/>
       <c r="M41" s="1" t="n">
-        <v>-24.016</v>
+        <v>0</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>-12.484</v>
+        <v>0</v>
       </c>
       <c r="O41" s="1" t="n">
-        <v>17.616</v>
+        <v>-6.4</v>
       </c>
       <c r="P41" s="1" t="n">
-        <v>9.76</v>
+        <v>-2.724</v>
       </c>
       <c r="Q41" s="1" t="n"/>
       <c r="R41" s="1" t="n"/>
       <c r="S41" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T41" s="1" t="n">
         <v>1</v>
@@ -2724,11 +2958,11 @@
     </row>
     <row r="42" spans="1:25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1" t="n"/>
       <c r="C42" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>-5.8</v>
@@ -2756,21 +2990,21 @@
       </c>
       <c r="L42" s="1" t="n"/>
       <c r="M42" s="1" t="n">
-        <v>24.016</v>
+        <v>0</v>
       </c>
       <c r="N42" s="1" t="n">
-        <v>-48.241</v>
+        <v>0</v>
       </c>
       <c r="O42" s="1" t="n">
-        <v>-29.816</v>
+        <v>-5.8</v>
       </c>
       <c r="P42" s="1" t="n">
-        <v>45.792</v>
+        <v>-2.449</v>
       </c>
       <c r="Q42" s="1" t="n"/>
       <c r="R42" s="1" t="n"/>
       <c r="S42" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T42" s="1" t="n">
         <v>1</v>
@@ -2793,11 +3027,11 @@
     </row>
     <row r="43" spans="1:25">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="n"/>
       <c r="C43" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D43" s="1" t="n">
         <v>-7</v>
@@ -2825,21 +3059,21 @@
       </c>
       <c r="L43" s="1" t="n"/>
       <c r="M43" s="1" t="n">
-        <v>24.016</v>
+        <v>0</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>-23.7185</v>
+        <v>0</v>
       </c>
       <c r="O43" s="1" t="n">
-        <v>-31.016</v>
+        <v>-7</v>
       </c>
       <c r="P43" s="1" t="n">
-        <v>20.7445</v>
+        <v>-2.974</v>
       </c>
       <c r="Q43" s="1" t="n"/>
       <c r="R43" s="1" t="n"/>
       <c r="S43" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T43" s="1" t="n">
         <v>1</v>
@@ -2862,11 +3096,11 @@
     </row>
     <row r="44" spans="1:25">
       <c r="A44" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="n"/>
       <c r="C44" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D44" s="1" t="n">
         <v>-7</v>
@@ -2894,21 +3128,21 @@
       </c>
       <c r="L44" s="1" t="n"/>
       <c r="M44" s="1" t="n">
-        <v>-24.016</v>
+        <v>0</v>
       </c>
       <c r="N44" s="1" t="n">
-        <v>11.8285</v>
+        <v>0</v>
       </c>
       <c r="O44" s="1" t="n">
-        <v>17.016</v>
+        <v>-7</v>
       </c>
       <c r="P44" s="1" t="n">
-        <v>-14.8025</v>
+        <v>-2.974</v>
       </c>
       <c r="Q44" s="1" t="n"/>
       <c r="R44" s="1" t="n"/>
       <c r="S44" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T44" s="1" t="n">
         <v>1</v>
@@ -2931,11 +3165,11 @@
     </row>
     <row r="45" spans="1:25">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="n"/>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>-4.5</v>
@@ -2963,21 +3197,21 @@
       </c>
       <c r="L45" s="1" t="n"/>
       <c r="M45" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="N45" s="1" t="n">
-        <v>-35.576</v>
+        <v>0.889</v>
       </c>
       <c r="O45" s="1" t="n">
-        <v>20.165</v>
+        <v>-16.3</v>
       </c>
       <c r="P45" s="1" t="n">
-        <v>39.576</v>
+        <v>3.111</v>
       </c>
       <c r="Q45" s="1" t="n"/>
       <c r="R45" s="1" t="n"/>
       <c r="S45" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T45" s="1" t="n">
         <v>4</v>
@@ -2986,7 +3220,7 @@
         <v>4</v>
       </c>
       <c r="V45" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W45" s="1" t="n">
         <v>0</v>
@@ -3000,11 +3234,11 @@
     </row>
     <row r="46" spans="1:25">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B46" s="1" t="n"/>
       <c r="C46" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>-4.5</v>
@@ -3032,21 +3266,21 @@
       </c>
       <c r="L46" s="1" t="n"/>
       <c r="M46" s="1" t="n">
-        <v>-48.275</v>
+        <v>-11.81</v>
       </c>
       <c r="N46" s="1" t="n">
-        <v>-36.506</v>
+        <v>-0.04100000000000004</v>
       </c>
       <c r="O46" s="1" t="n">
-        <v>43.775</v>
+        <v>7.309999999999999</v>
       </c>
       <c r="P46" s="1" t="n">
-        <v>40.506</v>
+        <v>4.041</v>
       </c>
       <c r="Q46" s="1" t="n"/>
       <c r="R46" s="1" t="n"/>
       <c r="S46" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T46" s="1" t="n">
         <v>4</v>
@@ -3055,7 +3289,7 @@
         <v>4</v>
       </c>
       <c r="V46" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W46" s="1" t="n">
         <v>0</v>
@@ -3069,11 +3303,11 @@
     </row>
     <row r="47" spans="1:25">
       <c r="A47" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B47" s="1" t="n"/>
       <c r="C47" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>-3.8</v>
@@ -3101,21 +3335,21 @@
       </c>
       <c r="L47" s="1" t="n"/>
       <c r="M47" s="1" t="n">
-        <v>-24.66</v>
+        <v>11.805</v>
       </c>
       <c r="N47" s="1" t="n">
-        <v>-35.697</v>
+        <v>0.768</v>
       </c>
       <c r="O47" s="1" t="n">
-        <v>20.86</v>
+        <v>-15.605</v>
       </c>
       <c r="P47" s="1" t="n">
-        <v>39.697</v>
+        <v>3.232</v>
       </c>
       <c r="Q47" s="1" t="n"/>
       <c r="R47" s="1" t="n"/>
       <c r="S47" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T47" s="1" t="n">
         <v>4</v>
@@ -3124,7 +3358,7 @@
         <v>4</v>
       </c>
       <c r="V47" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W47" s="1" t="n">
         <v>0</v>
@@ -3138,11 +3372,11 @@
     </row>
     <row r="48" spans="1:25">
       <c r="A48" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="n"/>
       <c r="C48" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>-3.8</v>
@@ -3170,21 +3404,21 @@
       </c>
       <c r="L48" s="1" t="n"/>
       <c r="M48" s="1" t="n">
-        <v>-48.27</v>
+        <v>-11.805</v>
       </c>
       <c r="N48" s="1" t="n">
-        <v>-36.627</v>
+        <v>-0.162</v>
       </c>
       <c r="O48" s="1" t="n">
-        <v>44.47000000000001</v>
+        <v>8.004999999999999</v>
       </c>
       <c r="P48" s="1" t="n">
-        <v>40.627</v>
+        <v>4.162</v>
       </c>
       <c r="Q48" s="1" t="n"/>
       <c r="R48" s="1" t="n"/>
       <c r="S48" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T48" s="1" t="n">
         <v>4</v>
@@ -3193,7 +3427,7 @@
         <v>4</v>
       </c>
       <c r="V48" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W48" s="1" t="n">
         <v>0</v>
@@ -3207,11 +3441,11 @@
     </row>
     <row r="49" spans="1:25">
       <c r="A49" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B49" s="1" t="n"/>
       <c r="C49" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>-4.548</v>
@@ -3239,21 +3473,21 @@
       </c>
       <c r="L49" s="1" t="n"/>
       <c r="M49" s="1" t="n">
-        <v>-48.255</v>
+        <v>-11.79</v>
       </c>
       <c r="N49" s="1" t="n">
-        <v>-37.073</v>
+        <v>-0.608</v>
       </c>
       <c r="O49" s="1" t="n">
-        <v>43.707</v>
+        <v>7.241999999999999</v>
       </c>
       <c r="P49" s="1" t="n">
-        <v>39.473</v>
+        <v>3.008</v>
       </c>
       <c r="Q49" s="1" t="n"/>
       <c r="R49" s="1" t="n"/>
       <c r="S49" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T49" s="1" t="n">
         <v>4</v>
@@ -3262,7 +3496,7 @@
         <v>4</v>
       </c>
       <c r="V49" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W49" s="1" t="n">
         <v>0</v>
@@ -3276,11 +3510,11 @@
     </row>
     <row r="50" spans="1:25">
       <c r="A50" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1" t="n"/>
       <c r="C50" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>-3.8</v>
@@ -3308,21 +3542,21 @@
       </c>
       <c r="L50" s="1" t="n"/>
       <c r="M50" s="1" t="n">
-        <v>-24.68</v>
+        <v>11.785</v>
       </c>
       <c r="N50" s="1" t="n">
-        <v>-36.143</v>
+        <v>0.322</v>
       </c>
       <c r="O50" s="1" t="n">
-        <v>20.88</v>
+        <v>-15.585</v>
       </c>
       <c r="P50" s="1" t="n">
-        <v>38.543</v>
+        <v>2.078</v>
       </c>
       <c r="Q50" s="1" t="n"/>
       <c r="R50" s="1" t="n"/>
       <c r="S50" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T50" s="1" t="n">
         <v>4</v>
@@ -3331,7 +3565,7 @@
         <v>4</v>
       </c>
       <c r="V50" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W50" s="1" t="n">
         <v>0</v>
@@ -3345,11 +3579,11 @@
     </row>
     <row r="51" spans="1:25">
       <c r="A51" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B51" s="1" t="n"/>
       <c r="C51" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>-5.929</v>
@@ -3391,7 +3625,7 @@
       <c r="Q51" s="1" t="n"/>
       <c r="R51" s="1" t="n"/>
       <c r="S51" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T51" s="1" t="n">
         <v>1</v>
@@ -3414,11 +3648,11 @@
     </row>
     <row r="52" spans="1:25">
       <c r="A52" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B52" s="1" t="n"/>
       <c r="C52" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D52" s="1" t="n">
         <v>6.069</v>
@@ -3460,7 +3694,7 @@
       <c r="Q52" s="1" t="n"/>
       <c r="R52" s="1" t="n"/>
       <c r="S52" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T52" s="1" t="n">
         <v>1</v>
@@ -3483,11 +3717,11 @@
     </row>
     <row r="53" spans="1:25">
       <c r="A53" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B53" s="1" t="n"/>
       <c r="C53" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>-3.31</v>
@@ -3515,21 +3749,21 @@
       </c>
       <c r="L53" s="1" t="n"/>
       <c r="M53" s="1" t="n">
-        <v>-13.802</v>
+        <v>0</v>
       </c>
       <c r="N53" s="1" t="n">
-        <v>-11.8</v>
+        <v>0</v>
       </c>
       <c r="O53" s="1" t="n">
-        <v>10.492</v>
+        <v>-3.31</v>
       </c>
       <c r="P53" s="1" t="n">
-        <v>16.939</v>
+        <v>5.139</v>
       </c>
       <c r="Q53" s="1" t="n"/>
       <c r="R53" s="1" t="n"/>
       <c r="S53" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T53" s="1" t="n">
         <v>1</v>
@@ -3541,7 +3775,7 @@
         <v>-6.901</v>
       </c>
       <c r="W53" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X53" s="1" t="n">
         <v>0</v>
@@ -3552,11 +3786,11 @@
     </row>
     <row r="54" spans="1:25">
       <c r="A54" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B54" s="1" t="n"/>
       <c r="C54" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>-5.65</v>
@@ -3584,21 +3818,21 @@
       </c>
       <c r="L54" s="1" t="n"/>
       <c r="M54" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N54" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O54" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P54" s="1" t="n">
-        <v>23.053</v>
+        <v>-13.412</v>
       </c>
       <c r="Q54" s="1" t="n"/>
       <c r="R54" s="1" t="n"/>
       <c r="S54" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T54" s="1" t="n">
         <v>4</v>
@@ -3607,7 +3841,7 @@
         <v>4</v>
       </c>
       <c r="V54" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W54" s="1" t="n">
         <v>0</v>
@@ -3621,11 +3855,11 @@
     </row>
     <row r="55" spans="1:25">
       <c r="A55" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B55" s="1" t="n"/>
       <c r="C55" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D55" s="1" t="n">
         <v>-5.65</v>
@@ -3653,21 +3887,21 @@
       </c>
       <c r="L55" s="1" t="n"/>
       <c r="M55" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N55" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O55" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P55" s="1" t="n">
-        <v>46.653</v>
+        <v>10.188</v>
       </c>
       <c r="Q55" s="1" t="n"/>
       <c r="R55" s="1" t="n"/>
       <c r="S55" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T55" s="1" t="n">
         <v>4</v>
@@ -3676,7 +3910,7 @@
         <v>4</v>
       </c>
       <c r="V55" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W55" s="1" t="n">
         <v>0</v>
@@ -3690,11 +3924,11 @@
     </row>
     <row r="56" spans="1:25">
       <c r="A56" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B56" s="1" t="n"/>
       <c r="C56" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D56" s="1" t="n">
         <v>-5.65</v>
@@ -3722,21 +3956,21 @@
       </c>
       <c r="L56" s="1" t="n"/>
       <c r="M56" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N56" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O56" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P56" s="1" t="n">
-        <v>20.653</v>
+        <v>-15.812</v>
       </c>
       <c r="Q56" s="1" t="n"/>
       <c r="R56" s="1" t="n"/>
       <c r="S56" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T56" s="1" t="n">
         <v>4</v>
@@ -3745,7 +3979,7 @@
         <v>4</v>
       </c>
       <c r="V56" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W56" s="1" t="n">
         <v>0</v>
@@ -3759,11 +3993,11 @@
     </row>
     <row r="57" spans="1:25">
       <c r="A57" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B57" s="1" t="n"/>
       <c r="C57" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>-5.65</v>
@@ -3791,21 +4025,21 @@
       </c>
       <c r="L57" s="1" t="n"/>
       <c r="M57" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N57" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O57" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P57" s="1" t="n">
-        <v>44.253</v>
+        <v>7.788000000000001</v>
       </c>
       <c r="Q57" s="1" t="n"/>
       <c r="R57" s="1" t="n"/>
       <c r="S57" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T57" s="1" t="n">
         <v>4</v>
@@ -3814,7 +4048,7 @@
         <v>4</v>
       </c>
       <c r="V57" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W57" s="1" t="n">
         <v>0</v>
@@ -3828,11 +4062,11 @@
     </row>
     <row r="58" spans="1:25">
       <c r="A58" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B58" s="1" t="n"/>
       <c r="C58" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="n">
         <v>-5.65</v>
@@ -3860,21 +4094,21 @@
       </c>
       <c r="L58" s="1" t="n"/>
       <c r="M58" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N58" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O58" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P58" s="1" t="n">
-        <v>20.053</v>
+        <v>-16.412</v>
       </c>
       <c r="Q58" s="1" t="n"/>
       <c r="R58" s="1" t="n"/>
       <c r="S58" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T58" s="1" t="n">
         <v>4</v>
@@ -3883,7 +4117,7 @@
         <v>4</v>
       </c>
       <c r="V58" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W58" s="1" t="n">
         <v>0</v>
@@ -3897,11 +4131,11 @@
     </row>
     <row r="59" spans="1:25">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B59" s="1" t="n"/>
       <c r="C59" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1" t="n">
         <v>-5.65</v>
@@ -3929,21 +4163,21 @@
       </c>
       <c r="L59" s="1" t="n"/>
       <c r="M59" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N59" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O59" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P59" s="1" t="n">
-        <v>43.653</v>
+        <v>7.188000000000001</v>
       </c>
       <c r="Q59" s="1" t="n"/>
       <c r="R59" s="1" t="n"/>
       <c r="S59" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T59" s="1" t="n">
         <v>4</v>
@@ -3952,7 +4186,7 @@
         <v>4</v>
       </c>
       <c r="V59" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W59" s="1" t="n">
         <v>0</v>
@@ -3966,11 +4200,11 @@
     </row>
     <row r="60" spans="1:25">
       <c r="A60" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B60" s="1" t="n"/>
       <c r="C60" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D60" s="1" t="n">
         <v>-5.65</v>
@@ -3998,21 +4232,21 @@
       </c>
       <c r="L60" s="1" t="n"/>
       <c r="M60" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N60" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O60" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P60" s="1" t="n">
-        <v>19.453</v>
+        <v>-17.012</v>
       </c>
       <c r="Q60" s="1" t="n"/>
       <c r="R60" s="1" t="n"/>
       <c r="S60" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T60" s="1" t="n">
         <v>4</v>
@@ -4021,7 +4255,7 @@
         <v>4</v>
       </c>
       <c r="V60" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W60" s="1" t="n">
         <v>0</v>
@@ -4035,11 +4269,11 @@
     </row>
     <row r="61" spans="1:25">
       <c r="A61" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B61" s="1" t="n"/>
       <c r="C61" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D61" s="1" t="n">
         <v>-5.65</v>
@@ -4067,21 +4301,21 @@
       </c>
       <c r="L61" s="1" t="n"/>
       <c r="M61" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N61" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O61" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>43.053</v>
+        <v>6.588000000000001</v>
       </c>
       <c r="Q61" s="1" t="n"/>
       <c r="R61" s="1" t="n"/>
       <c r="S61" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T61" s="1" t="n">
         <v>4</v>
@@ -4090,7 +4324,7 @@
         <v>4</v>
       </c>
       <c r="V61" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W61" s="1" t="n">
         <v>0</v>
@@ -4104,11 +4338,11 @@
     </row>
     <row r="62" spans="1:25">
       <c r="A62" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B62" s="1" t="n"/>
       <c r="C62" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D62" s="1" t="n">
         <v>-5.65</v>
@@ -4136,21 +4370,21 @@
       </c>
       <c r="L62" s="1" t="n"/>
       <c r="M62" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N62" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O62" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P62" s="1" t="n">
-        <v>18.853</v>
+        <v>-17.612</v>
       </c>
       <c r="Q62" s="1" t="n"/>
       <c r="R62" s="1" t="n"/>
       <c r="S62" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T62" s="1" t="n">
         <v>4</v>
@@ -4159,7 +4393,7 @@
         <v>4</v>
       </c>
       <c r="V62" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W62" s="1" t="n">
         <v>0</v>
@@ -4173,11 +4407,11 @@
     </row>
     <row r="63" spans="1:25">
       <c r="A63" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B63" s="1" t="n"/>
       <c r="C63" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D63" s="1" t="n">
         <v>-5.65</v>
@@ -4205,21 +4439,21 @@
       </c>
       <c r="L63" s="1" t="n"/>
       <c r="M63" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N63" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O63" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P63" s="1" t="n">
-        <v>42.453</v>
+        <v>5.988</v>
       </c>
       <c r="Q63" s="1" t="n"/>
       <c r="R63" s="1" t="n"/>
       <c r="S63" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T63" s="1" t="n">
         <v>4</v>
@@ -4228,7 +4462,7 @@
         <v>4</v>
       </c>
       <c r="V63" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W63" s="1" t="n">
         <v>0</v>
@@ -4242,11 +4476,11 @@
     </row>
     <row r="64" spans="1:25">
       <c r="A64" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B64" s="1" t="n"/>
       <c r="C64" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D64" s="1" t="n">
         <v>1</v>
@@ -4274,21 +4508,21 @@
       </c>
       <c r="L64" s="1" t="n"/>
       <c r="M64" s="1" t="n">
-        <v>-5.579972</v>
+        <v>0</v>
       </c>
       <c r="N64" s="1" t="n">
-        <v>-5.581528</v>
+        <v>0</v>
       </c>
       <c r="O64" s="1" t="n">
-        <v>6.579972</v>
+        <v>1</v>
       </c>
       <c r="P64" s="1" t="n">
-        <v>3.381528</v>
+        <v>-2.2</v>
       </c>
       <c r="Q64" s="1" t="n"/>
       <c r="R64" s="1" t="n"/>
       <c r="S64" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T64" s="1" t="n">
         <v>2</v>
@@ -4311,11 +4545,11 @@
     </row>
     <row r="65" spans="1:25">
       <c r="A65" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B65" s="1" t="n"/>
       <c r="C65" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D65" s="1" t="n">
         <v>-7</v>
@@ -4343,21 +4577,21 @@
       </c>
       <c r="L65" s="1" t="n"/>
       <c r="M65" s="1" t="n">
-        <v>-48.473</v>
+        <v>-12.008</v>
       </c>
       <c r="N65" s="1" t="n">
-        <v>48.342</v>
+        <v>48.234</v>
       </c>
       <c r="O65" s="1" t="n">
-        <v>41.473</v>
+        <v>5.007999999999999</v>
       </c>
       <c r="P65" s="1" t="n">
-        <v>-44.691</v>
+        <v>-44.583</v>
       </c>
       <c r="Q65" s="1" t="n"/>
       <c r="R65" s="1" t="n"/>
       <c r="S65" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T65" s="1" t="n">
         <v>4</v>
@@ -4366,10 +4600,10 @@
         <v>1</v>
       </c>
       <c r="V65" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W65" s="1" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="X65" s="1" t="n">
         <v>24.31</v>
@@ -4380,11 +4614,11 @@
     </row>
     <row r="66" spans="1:25">
       <c r="A66" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B66" s="1" t="n"/>
       <c r="C66" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D66" s="1" t="n">
         <v>4</v>
@@ -4412,21 +4646,21 @@
       </c>
       <c r="L66" s="1" t="n"/>
       <c r="M66" s="1" t="n">
-        <v>-11.2</v>
+        <v>0</v>
       </c>
       <c r="N66" s="1" t="n">
-        <v>-7.462</v>
+        <v>0</v>
       </c>
       <c r="O66" s="1" t="n">
-        <v>15.2</v>
+        <v>4</v>
       </c>
       <c r="P66" s="1" t="n">
-        <v>12.462</v>
+        <v>5</v>
       </c>
       <c r="Q66" s="1" t="n"/>
       <c r="R66" s="1" t="n"/>
       <c r="S66" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T66" s="1" t="n">
         <v>1</v>
@@ -4449,11 +4683,11 @@
     </row>
     <row r="67" spans="1:25">
       <c r="A67" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B67" s="1" t="n"/>
       <c r="C67" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D67" s="1" t="n">
         <v>4</v>
@@ -4481,21 +4715,21 @@
       </c>
       <c r="L67" s="1" t="n"/>
       <c r="M67" s="1" t="n">
-        <v>11.158</v>
+        <v>0</v>
       </c>
       <c r="N67" s="1" t="n">
-        <v>-7.434</v>
+        <v>0</v>
       </c>
       <c r="O67" s="1" t="n">
-        <v>-7.157999999999999</v>
+        <v>4</v>
       </c>
       <c r="P67" s="1" t="n">
-        <v>3.884</v>
+        <v>-3.55</v>
       </c>
       <c r="Q67" s="1" t="n"/>
       <c r="R67" s="1" t="n"/>
       <c r="S67" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T67" s="1" t="n">
         <v>1</v>
@@ -4518,11 +4752,11 @@
     </row>
     <row r="68" spans="1:25">
       <c r="A68" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B68" s="1" t="n"/>
       <c r="C68" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>-8.074</v>
@@ -4550,21 +4784,21 @@
       </c>
       <c r="L68" s="1" t="n"/>
       <c r="M68" s="1" t="n">
-        <v>-48.1</v>
+        <v>-11.635</v>
       </c>
       <c r="N68" s="1" t="n">
-        <v>-36.529</v>
+        <v>-0.064</v>
       </c>
       <c r="O68" s="1" t="n">
-        <v>40.026</v>
+        <v>3.561</v>
       </c>
       <c r="P68" s="1" t="n">
-        <v>36.529</v>
+        <v>0.064</v>
       </c>
       <c r="Q68" s="1" t="n"/>
       <c r="R68" s="1" t="n"/>
       <c r="S68" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T68" s="1" t="n">
         <v>4</v>
@@ -4573,7 +4807,7 @@
         <v>4</v>
       </c>
       <c r="V68" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W68" s="1" t="n">
         <v>0</v>
@@ -4587,11 +4821,11 @@
     </row>
     <row r="69" spans="1:25">
       <c r="A69" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B69" s="1" t="n"/>
       <c r="C69" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>8.000999999999999</v>
@@ -4619,21 +4853,21 @@
       </c>
       <c r="L69" s="1" t="n"/>
       <c r="M69" s="1" t="n">
-        <v>-24.829</v>
+        <v>11.636</v>
       </c>
       <c r="N69" s="1" t="n">
-        <v>-36.4</v>
+        <v>0.065</v>
       </c>
       <c r="O69" s="1" t="n">
-        <v>32.83</v>
+        <v>-3.635</v>
       </c>
       <c r="P69" s="1" t="n">
-        <v>36.4</v>
+        <v>-0.065</v>
       </c>
       <c r="Q69" s="1" t="n"/>
       <c r="R69" s="1" t="n"/>
       <c r="S69" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T69" s="1" t="n">
         <v>4</v>
@@ -4642,7 +4876,7 @@
         <v>4</v>
       </c>
       <c r="V69" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W69" s="1" t="n">
         <v>0</v>
@@ -4656,11 +4890,11 @@
     </row>
     <row r="70" spans="1:25">
       <c r="A70" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B70" s="1" t="n"/>
       <c r="C70" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>2.674</v>
@@ -4688,21 +4922,21 @@
       </c>
       <c r="L70" s="1" t="n"/>
       <c r="M70" s="1" t="n">
-        <v>13.816</v>
+        <v>0</v>
       </c>
       <c r="N70" s="1" t="n">
-        <v>-11.8</v>
+        <v>0</v>
       </c>
       <c r="O70" s="1" t="n">
-        <v>-11.142</v>
+        <v>2.674</v>
       </c>
       <c r="P70" s="1" t="n">
-        <v>16.091</v>
+        <v>4.291</v>
       </c>
       <c r="Q70" s="1" t="n"/>
       <c r="R70" s="1" t="n"/>
       <c r="S70" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T70" s="1" t="n">
         <v>1</v>
@@ -4714,7 +4948,7 @@
         <v>6.908</v>
       </c>
       <c r="W70" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X70" s="1" t="n">
         <v>8.279999999999999</v>
@@ -4725,11 +4959,11 @@
     </row>
     <row r="71" spans="1:25">
       <c r="A71" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B71" s="1" t="n"/>
       <c r="C71" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>-2.79</v>
@@ -4757,21 +4991,21 @@
       </c>
       <c r="L71" s="1" t="n"/>
       <c r="M71" s="1" t="n">
-        <v>-45.299</v>
+        <v>-8.834</v>
       </c>
       <c r="N71" s="1" t="n">
-        <v>48.822</v>
+        <v>48.714</v>
       </c>
       <c r="O71" s="1" t="n">
-        <v>42.509</v>
+        <v>6.044</v>
       </c>
       <c r="P71" s="1" t="n">
-        <v>-41.544</v>
+        <v>-41.436</v>
       </c>
       <c r="Q71" s="1" t="n"/>
       <c r="R71" s="1" t="n"/>
       <c r="S71" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T71" s="1" t="n">
         <v>4</v>
@@ -4780,10 +5014,10 @@
         <v>1</v>
       </c>
       <c r="V71" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W71" s="1" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="X71" s="1" t="n">
         <v>24.31</v>
@@ -4794,11 +5028,11 @@
     </row>
     <row r="72" spans="1:25">
       <c r="A72" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B72" s="1" t="n"/>
       <c r="C72" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>-3.099</v>
@@ -4826,21 +5060,21 @@
       </c>
       <c r="L72" s="1" t="n"/>
       <c r="M72" s="1" t="n">
-        <v>-39.641</v>
+        <v>-3.176</v>
       </c>
       <c r="N72" s="1" t="n">
-        <v>48.952</v>
+        <v>48.844</v>
       </c>
       <c r="O72" s="1" t="n">
-        <v>36.542</v>
+        <v>0.07699999999999996</v>
       </c>
       <c r="P72" s="1" t="n">
-        <v>-40.452</v>
+        <v>-40.344</v>
       </c>
       <c r="Q72" s="1" t="n"/>
       <c r="R72" s="1" t="n"/>
       <c r="S72" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T72" s="1" t="n">
         <v>4</v>
@@ -4849,10 +5083,10 @@
         <v>1</v>
       </c>
       <c r="V72" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W72" s="1" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="X72" s="1" t="n">
         <v>24.31</v>
@@ -4863,11 +5097,11 @@
     </row>
     <row r="73" spans="1:25">
       <c r="A73" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B73" s="1" t="n"/>
       <c r="C73" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>3.147</v>
@@ -4895,21 +5129,21 @@
       </c>
       <c r="L73" s="1" t="n"/>
       <c r="M73" s="1" t="n">
-        <v>-27.631</v>
+        <v>8.834</v>
       </c>
       <c r="N73" s="1" t="n">
-        <v>48.822</v>
+        <v>48.714</v>
       </c>
       <c r="O73" s="1" t="n">
-        <v>30.778</v>
+        <v>-5.686999999999999</v>
       </c>
       <c r="P73" s="1" t="n">
-        <v>-42.736</v>
+        <v>-42.628</v>
       </c>
       <c r="Q73" s="1" t="n"/>
       <c r="R73" s="1" t="n"/>
       <c r="S73" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T73" s="1" t="n">
         <v>4</v>
@@ -4918,10 +5152,10 @@
         <v>1</v>
       </c>
       <c r="V73" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W73" s="1" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="X73" s="1" t="n">
         <v>24.31</v>
@@ -4932,11 +5166,11 @@
     </row>
     <row r="74" spans="1:25">
       <c r="A74" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B74" s="1" t="n"/>
       <c r="C74" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>3.701</v>
@@ -4964,21 +5198,21 @@
       </c>
       <c r="L74" s="1" t="n"/>
       <c r="M74" s="1" t="n">
-        <v>-33.289</v>
+        <v>3.176</v>
       </c>
       <c r="N74" s="1" t="n">
-        <v>48.952</v>
+        <v>48.844</v>
       </c>
       <c r="O74" s="1" t="n">
-        <v>36.99</v>
+        <v>0.5249999999999999</v>
       </c>
       <c r="P74" s="1" t="n">
-        <v>-40.452</v>
+        <v>-40.344</v>
       </c>
       <c r="Q74" s="1" t="n"/>
       <c r="R74" s="1" t="n"/>
       <c r="S74" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T74" s="1" t="n">
         <v>4</v>
@@ -4987,10 +5221,10 @@
         <v>1</v>
       </c>
       <c r="V74" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W74" s="1" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="X74" s="1" t="n">
         <v>24.31</v>
@@ -5001,11 +5235,11 @@
     </row>
     <row r="75" spans="1:25">
       <c r="A75" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B75" s="1" t="n"/>
       <c r="C75" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D75" s="1" t="n">
         <v>-5.65</v>
@@ -5033,21 +5267,21 @@
       </c>
       <c r="L75" s="1" t="n"/>
       <c r="M75" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N75" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O75" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P75" s="1" t="n">
-        <v>18.253</v>
+        <v>-18.212</v>
       </c>
       <c r="Q75" s="1" t="n"/>
       <c r="R75" s="1" t="n"/>
       <c r="S75" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T75" s="1" t="n">
         <v>4</v>
@@ -5056,7 +5290,7 @@
         <v>4</v>
       </c>
       <c r="V75" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W75" s="1" t="n">
         <v>0</v>
@@ -5070,11 +5304,11 @@
     </row>
     <row r="76" spans="1:25">
       <c r="A76" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B76" s="1" t="n"/>
       <c r="C76" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D76" s="1" t="n">
         <v>-5.65</v>
@@ -5102,21 +5336,21 @@
       </c>
       <c r="L76" s="1" t="n"/>
       <c r="M76" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N76" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O76" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P76" s="1" t="n">
-        <v>41.853</v>
+        <v>5.388000000000001</v>
       </c>
       <c r="Q76" s="1" t="n"/>
       <c r="R76" s="1" t="n"/>
       <c r="S76" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T76" s="1" t="n">
         <v>4</v>
@@ -5125,7 +5359,7 @@
         <v>4</v>
       </c>
       <c r="V76" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W76" s="1" t="n">
         <v>0</v>
@@ -5139,11 +5373,11 @@
     </row>
     <row r="77" spans="1:25">
       <c r="A77" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B77" s="1" t="n"/>
       <c r="C77" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D77" s="1" t="n">
         <v>-5.65</v>
@@ -5171,21 +5405,21 @@
       </c>
       <c r="L77" s="1" t="n"/>
       <c r="M77" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N77" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O77" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P77" s="1" t="n">
-        <v>24.259</v>
+        <v>-12.206</v>
       </c>
       <c r="Q77" s="1" t="n"/>
       <c r="R77" s="1" t="n"/>
       <c r="S77" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T77" s="1" t="n">
         <v>4</v>
@@ -5194,7 +5428,7 @@
         <v>4</v>
       </c>
       <c r="V77" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W77" s="1" t="n">
         <v>0</v>
@@ -5208,11 +5442,11 @@
     </row>
     <row r="78" spans="1:25">
       <c r="A78" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B78" s="1" t="n"/>
       <c r="C78" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>-5.65</v>
@@ -5240,21 +5474,21 @@
       </c>
       <c r="L78" s="1" t="n"/>
       <c r="M78" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N78" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O78" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P78" s="1" t="n">
-        <v>47.859</v>
+        <v>11.394</v>
       </c>
       <c r="Q78" s="1" t="n"/>
       <c r="R78" s="1" t="n"/>
       <c r="S78" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T78" s="1" t="n">
         <v>4</v>
@@ -5263,7 +5497,7 @@
         <v>4</v>
       </c>
       <c r="V78" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W78" s="1" t="n">
         <v>0</v>
@@ -5277,11 +5511,11 @@
     </row>
     <row r="79" spans="1:25">
       <c r="A79" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B79" s="1" t="n"/>
       <c r="C79" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>-7.274</v>
@@ -5309,21 +5543,21 @@
       </c>
       <c r="L79" s="1" t="n"/>
       <c r="M79" s="1" t="n">
-        <v>-28.73</v>
+        <v>0</v>
       </c>
       <c r="N79" s="1" t="n">
-        <v>104.682</v>
+        <v>0</v>
       </c>
       <c r="O79" s="1" t="n">
-        <v>21.456</v>
+        <v>-7.274</v>
       </c>
       <c r="P79" s="1" t="n">
-        <v>-94.7</v>
+        <v>9.981999999999999</v>
       </c>
       <c r="Q79" s="1" t="n"/>
       <c r="R79" s="1" t="n"/>
       <c r="S79" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T79" s="1" t="n">
         <v>8</v>
@@ -5335,7 +5569,7 @@
         <v>-0.015</v>
       </c>
       <c r="W79" s="1" t="n">
-        <v>52.341</v>
+        <v>51.891</v>
       </c>
       <c r="X79" s="1" t="n">
         <v>8.199999999999999</v>
@@ -5346,11 +5580,11 @@
     </row>
     <row r="80" spans="1:25">
       <c r="A80" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B80" s="1" t="n"/>
       <c r="C80" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>-3.22</v>
@@ -5378,21 +5612,21 @@
       </c>
       <c r="L80" s="1" t="n"/>
       <c r="M80" s="1" t="n">
-        <v>-48.255</v>
+        <v>-11.79</v>
       </c>
       <c r="N80" s="1" t="n">
-        <v>-37.073</v>
+        <v>-0.608</v>
       </c>
       <c r="O80" s="1" t="n">
-        <v>45.035</v>
+        <v>8.569999999999999</v>
       </c>
       <c r="P80" s="1" t="n">
-        <v>39.473</v>
+        <v>3.008</v>
       </c>
       <c r="Q80" s="1" t="n"/>
       <c r="R80" s="1" t="n"/>
       <c r="S80" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T80" s="1" t="n">
         <v>4</v>
@@ -5401,7 +5635,7 @@
         <v>4</v>
       </c>
       <c r="V80" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W80" s="1" t="n">
         <v>0</v>
@@ -5415,11 +5649,11 @@
     </row>
     <row r="81" spans="1:25">
       <c r="A81" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B81" s="1" t="n"/>
       <c r="C81" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>-2.558</v>
@@ -5447,21 +5681,21 @@
       </c>
       <c r="L81" s="1" t="n"/>
       <c r="M81" s="1" t="n">
-        <v>-24.68</v>
+        <v>11.785</v>
       </c>
       <c r="N81" s="1" t="n">
-        <v>-36.143</v>
+        <v>0.322</v>
       </c>
       <c r="O81" s="1" t="n">
-        <v>22.122</v>
+        <v>-14.343</v>
       </c>
       <c r="P81" s="1" t="n">
-        <v>38.543</v>
+        <v>2.078</v>
       </c>
       <c r="Q81" s="1" t="n"/>
       <c r="R81" s="1" t="n"/>
       <c r="S81" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T81" s="1" t="n">
         <v>4</v>
@@ -5470,7 +5704,7 @@
         <v>4</v>
       </c>
       <c r="V81" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W81" s="1" t="n">
         <v>0</v>
@@ -5484,11 +5718,11 @@
     </row>
     <row r="82" spans="1:25">
       <c r="A82" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B82" s="1" t="n"/>
       <c r="C82" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D82" s="1" t="n">
         <v>-5.65</v>
@@ -5516,21 +5750,21 @@
       </c>
       <c r="L82" s="1" t="n"/>
       <c r="M82" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N82" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O82" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P82" s="1" t="n">
-        <v>23.659</v>
+        <v>-12.806</v>
       </c>
       <c r="Q82" s="1" t="n"/>
       <c r="R82" s="1" t="n"/>
       <c r="S82" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T82" s="1" t="n">
         <v>4</v>
@@ -5539,7 +5773,7 @@
         <v>4</v>
       </c>
       <c r="V82" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W82" s="1" t="n">
         <v>0</v>
@@ -5553,11 +5787,11 @@
     </row>
     <row r="83" spans="1:25">
       <c r="A83" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B83" s="1" t="n"/>
       <c r="C83" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D83" s="1" t="n">
         <v>-5.65</v>
@@ -5585,21 +5819,21 @@
       </c>
       <c r="L83" s="1" t="n"/>
       <c r="M83" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N83" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O83" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P83" s="1" t="n">
-        <v>47.259</v>
+        <v>10.794</v>
       </c>
       <c r="Q83" s="1" t="n"/>
       <c r="R83" s="1" t="n"/>
       <c r="S83" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T83" s="1" t="n">
         <v>4</v>
@@ -5608,7 +5842,7 @@
         <v>4</v>
       </c>
       <c r="V83" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W83" s="1" t="n">
         <v>0</v>
@@ -5622,11 +5856,11 @@
     </row>
     <row r="84" spans="1:25">
       <c r="A84" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B84" s="1" t="n"/>
       <c r="C84" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D84" s="1" t="n">
         <v>-5.65</v>
@@ -5654,21 +5888,21 @@
       </c>
       <c r="L84" s="1" t="n"/>
       <c r="M84" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N84" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O84" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P84" s="1" t="n">
-        <v>21.253</v>
+        <v>-15.212</v>
       </c>
       <c r="Q84" s="1" t="n"/>
       <c r="R84" s="1" t="n"/>
       <c r="S84" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T84" s="1" t="n">
         <v>4</v>
@@ -5677,7 +5911,7 @@
         <v>4</v>
       </c>
       <c r="V84" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W84" s="1" t="n">
         <v>0</v>
@@ -5691,11 +5925,11 @@
     </row>
     <row r="85" spans="1:25">
       <c r="A85" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B85" s="1" t="n"/>
       <c r="C85" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D85" s="1" t="n">
         <v>-5.65</v>
@@ -5723,21 +5957,21 @@
       </c>
       <c r="L85" s="1" t="n"/>
       <c r="M85" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N85" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O85" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P85" s="1" t="n">
-        <v>44.853</v>
+        <v>8.388000000000002</v>
       </c>
       <c r="Q85" s="1" t="n"/>
       <c r="R85" s="1" t="n"/>
       <c r="S85" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T85" s="1" t="n">
         <v>4</v>
@@ -5746,7 +5980,7 @@
         <v>4</v>
       </c>
       <c r="V85" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W85" s="1" t="n">
         <v>0</v>
@@ -5760,11 +5994,11 @@
     </row>
     <row r="86" spans="1:25">
       <c r="A86" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B86" s="1" t="n"/>
       <c r="C86" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D86" s="1" t="n">
         <v>-2.442</v>
@@ -5806,7 +6040,7 @@
       <c r="Q86" s="1" t="n"/>
       <c r="R86" s="1" t="n"/>
       <c r="S86" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T86" s="1" t="n">
         <v>1</v>
@@ -5829,11 +6063,11 @@
     </row>
     <row r="87" spans="1:25">
       <c r="A87" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B87" s="1" t="n"/>
       <c r="C87" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>-2.442</v>
@@ -5861,21 +6095,21 @@
       </c>
       <c r="L87" s="1" t="n"/>
       <c r="M87" s="1" t="n">
-        <v>-24.726</v>
+        <v>0</v>
       </c>
       <c r="N87" s="1" t="n">
-        <v>98.134</v>
+        <v>0</v>
       </c>
       <c r="O87" s="1" t="n">
-        <v>22.284</v>
+        <v>-2.442</v>
       </c>
       <c r="P87" s="1" t="n">
-        <v>-86.113</v>
+        <v>12.021</v>
       </c>
       <c r="Q87" s="1" t="n"/>
       <c r="R87" s="1" t="n"/>
       <c r="S87" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T87" s="1" t="n">
         <v>7</v>
@@ -5898,11 +6132,11 @@
     </row>
     <row r="88" spans="1:25">
       <c r="A88" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B88" s="1" t="n"/>
       <c r="C88" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>-2.442</v>
@@ -5944,7 +6178,7 @@
       <c r="Q88" s="1" t="n"/>
       <c r="R88" s="1" t="n"/>
       <c r="S88" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="T88" s="1" t="n">
         <v>1</v>
@@ -5967,11 +6201,11 @@
     </row>
     <row r="89" spans="1:25">
       <c r="A89" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B89" s="1" t="n"/>
       <c r="C89" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D89" s="1" t="n">
         <v>-1.4</v>
@@ -5999,21 +6233,21 @@
       </c>
       <c r="L89" s="1" t="n"/>
       <c r="M89" s="1" t="n">
-        <v>-40.948</v>
+        <v>-4.483</v>
       </c>
       <c r="N89" s="1" t="n">
-        <v>-24.589</v>
+        <v>11.876</v>
       </c>
       <c r="O89" s="1" t="n">
-        <v>39.548</v>
+        <v>3.083</v>
       </c>
       <c r="P89" s="1" t="n">
-        <v>16.189</v>
+        <v>-20.276</v>
       </c>
       <c r="Q89" s="1" t="n"/>
       <c r="R89" s="1" t="n"/>
       <c r="S89" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T89" s="1" t="n">
         <v>4</v>
@@ -6022,7 +6256,7 @@
         <v>4</v>
       </c>
       <c r="V89" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W89" s="1" t="n">
         <v>0</v>
@@ -6036,11 +6270,11 @@
     </row>
     <row r="90" spans="1:25">
       <c r="A90" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B90" s="1" t="n"/>
       <c r="C90" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>1.4</v>
@@ -6068,21 +6302,21 @@
       </c>
       <c r="L90" s="1" t="n"/>
       <c r="M90" s="1" t="n">
-        <v>-31.982</v>
+        <v>4.483</v>
       </c>
       <c r="N90" s="1" t="n">
-        <v>-48.332</v>
+        <v>-11.867</v>
       </c>
       <c r="O90" s="1" t="n">
-        <v>33.382</v>
+        <v>-3.083</v>
       </c>
       <c r="P90" s="1" t="n">
-        <v>38.732</v>
+        <v>2.267000000000001</v>
       </c>
       <c r="Q90" s="1" t="n"/>
       <c r="R90" s="1" t="n"/>
       <c r="S90" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T90" s="1" t="n">
         <v>4</v>
@@ -6091,7 +6325,7 @@
         <v>4</v>
       </c>
       <c r="V90" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W90" s="1" t="n">
         <v>0</v>
@@ -6105,11 +6339,11 @@
     </row>
     <row r="91" spans="1:25">
       <c r="A91" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B91" s="1" t="n"/>
       <c r="C91" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>-5.65</v>
@@ -6137,21 +6371,21 @@
       </c>
       <c r="L91" s="1" t="n"/>
       <c r="M91" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N91" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O91" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P91" s="1" t="n">
-        <v>24.859</v>
+        <v>-11.606</v>
       </c>
       <c r="Q91" s="1" t="n"/>
       <c r="R91" s="1" t="n"/>
       <c r="S91" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T91" s="1" t="n">
         <v>4</v>
@@ -6160,7 +6394,7 @@
         <v>4</v>
       </c>
       <c r="V91" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W91" s="1" t="n">
         <v>0</v>
@@ -6174,11 +6408,11 @@
     </row>
     <row r="92" spans="1:25">
       <c r="A92" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B92" s="1" t="n"/>
       <c r="C92" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D92" s="1" t="n">
         <v>-5.65</v>
@@ -6206,21 +6440,21 @@
       </c>
       <c r="L92" s="1" t="n"/>
       <c r="M92" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N92" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O92" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P92" s="1" t="n">
-        <v>48.459</v>
+        <v>11.994</v>
       </c>
       <c r="Q92" s="1" t="n"/>
       <c r="R92" s="1" t="n"/>
       <c r="S92" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T92" s="1" t="n">
         <v>4</v>
@@ -6229,7 +6463,7 @@
         <v>4</v>
       </c>
       <c r="V92" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W92" s="1" t="n">
         <v>0</v>
@@ -6243,11 +6477,11 @@
     </row>
     <row r="93" spans="1:25">
       <c r="A93" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B93" s="1" t="n"/>
       <c r="C93" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D93" s="1" t="n">
         <v>-5.65</v>
@@ -6275,21 +6509,21 @@
       </c>
       <c r="L93" s="1" t="n"/>
       <c r="M93" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N93" s="1" t="n">
-        <v>-24.665</v>
+        <v>11.8</v>
       </c>
       <c r="O93" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P93" s="1" t="n">
-        <v>22.453</v>
+        <v>-14.012</v>
       </c>
       <c r="Q93" s="1" t="n"/>
       <c r="R93" s="1" t="n"/>
       <c r="S93" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T93" s="1" t="n">
         <v>4</v>
@@ -6298,7 +6532,7 @@
         <v>4</v>
       </c>
       <c r="V93" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W93" s="1" t="n">
         <v>0</v>
@@ -6312,11 +6546,11 @@
     </row>
     <row r="94" spans="1:25">
       <c r="A94" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B94" s="1" t="n"/>
       <c r="C94" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D94" s="1" t="n">
         <v>-5.65</v>
@@ -6344,21 +6578,21 @@
       </c>
       <c r="L94" s="1" t="n"/>
       <c r="M94" s="1" t="n">
-        <v>-36.465</v>
+        <v>0</v>
       </c>
       <c r="N94" s="1" t="n">
-        <v>-48.265</v>
+        <v>-11.8</v>
       </c>
       <c r="O94" s="1" t="n">
-        <v>30.815</v>
+        <v>-5.65</v>
       </c>
       <c r="P94" s="1" t="n">
-        <v>46.053</v>
+        <v>9.588000000000001</v>
       </c>
       <c r="Q94" s="1" t="n"/>
       <c r="R94" s="1" t="n"/>
       <c r="S94" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T94" s="1" t="n">
         <v>4</v>
@@ -6367,7 +6601,7 @@
         <v>4</v>
       </c>
       <c r="V94" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W94" s="1" t="n">
         <v>0</v>
@@ -6381,11 +6615,11 @@
     </row>
     <row r="95" spans="1:25">
       <c r="A95" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B95" s="1" t="n"/>
       <c r="C95" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D95" s="1" t="n">
         <v>6</v>
@@ -6413,21 +6647,21 @@
       </c>
       <c r="L95" s="1" t="n"/>
       <c r="M95" s="1" t="n">
-        <v>-95.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="N95" s="1" t="n">
-        <v>104.11</v>
+        <v>0</v>
       </c>
       <c r="O95" s="1" t="n">
-        <v>101.1</v>
+        <v>6</v>
       </c>
       <c r="P95" s="1" t="n">
-        <v>-93.41</v>
+        <v>10.7</v>
       </c>
       <c r="Q95" s="1" t="n"/>
       <c r="R95" s="1" t="n"/>
       <c r="S95" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T95" s="1" t="n">
         <v>1</v>
@@ -6450,11 +6684,11 @@
     </row>
     <row r="96" spans="1:25">
       <c r="A96" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B96" s="1" t="n"/>
       <c r="C96" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D96" s="1" t="n">
         <v>6</v>
@@ -6496,7 +6730,7 @@
       <c r="Q96" s="1" t="n"/>
       <c r="R96" s="1" t="n"/>
       <c r="S96" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T96" s="1" t="n">
         <v>1</v>
@@ -6519,11 +6753,11 @@
     </row>
     <row r="97" spans="1:25">
       <c r="A97" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B97" s="1" t="n"/>
       <c r="C97" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D97" s="1" t="n">
         <v>6</v>
@@ -6565,7 +6799,7 @@
       <c r="Q97" s="1" t="n"/>
       <c r="R97" s="1" t="n"/>
       <c r="S97" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T97" s="1" t="n">
         <v>1</v>
@@ -6588,11 +6822,11 @@
     </row>
     <row r="98" spans="1:25">
       <c r="A98" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B98" s="1" t="n"/>
       <c r="C98" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D98" s="1" t="n">
         <v>6</v>
@@ -6620,21 +6854,21 @@
       </c>
       <c r="L98" s="1" t="n"/>
       <c r="M98" s="1" t="n">
-        <v>-95.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="N98" s="1" t="n">
-        <v>-109.66</v>
+        <v>0</v>
       </c>
       <c r="O98" s="1" t="n">
-        <v>101.1</v>
+        <v>6</v>
       </c>
       <c r="P98" s="1" t="n">
-        <v>120.36</v>
+        <v>10.7</v>
       </c>
       <c r="Q98" s="1" t="n"/>
       <c r="R98" s="1" t="n"/>
       <c r="S98" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T98" s="1" t="n">
         <v>1</v>
@@ -6657,11 +6891,11 @@
     </row>
     <row r="99" spans="1:25">
       <c r="A99" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B99" s="1" t="n"/>
       <c r="C99" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D99" s="1" t="n">
         <v>-9.300000000000001</v>
@@ -6689,21 +6923,21 @@
       </c>
       <c r="L99" s="1" t="n"/>
       <c r="M99" s="1" t="n">
-        <v>-56.3</v>
+        <v>0</v>
       </c>
       <c r="N99" s="1" t="n">
-        <v>-49.05</v>
+        <v>0</v>
       </c>
       <c r="O99" s="1" t="n">
-        <v>47</v>
+        <v>-9.300000000000001</v>
       </c>
       <c r="P99" s="1" t="n">
-        <v>44.65</v>
+        <v>-4.4</v>
       </c>
       <c r="Q99" s="1" t="n"/>
       <c r="R99" s="1" t="n"/>
       <c r="S99" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T99" s="1" t="n">
         <v>2</v>
@@ -6712,10 +6946,10 @@
         <v>19</v>
       </c>
       <c r="V99" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W99" s="1" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="X99" s="1" t="n">
         <v>112.6</v>

</xml_diff>